<commit_message>
Enhance README documentation for PA and Per Diem shift assignments. Add detailed notes on shift limits and assignment rules. Introduce new JSON file for updated shifts and improve date parsing in PAList component. Refactor scheduling service to include enhanced weekend shift balancing and load distribution logic. Update PerDiem model to include max shifts property.
</commit_message>
<xml_diff>
--- a/TemplateFile/Template.xlsx
+++ b/TemplateFile/Template.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\source\pa_scheduler\TestFile\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\source\pa_scheduler\TemplateFile\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="16935"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="16935" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="RequestedWorkDay" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="22">
   <si>
     <t>Date</t>
   </si>
@@ -49,6 +49,54 @@
   </si>
   <si>
     <t>Dates Available to Work End</t>
+  </si>
+  <si>
+    <t>Jun (A1)</t>
+  </si>
+  <si>
+    <t>Jay (A2)</t>
+  </si>
+  <si>
+    <t>Colleen (A3)</t>
+  </si>
+  <si>
+    <t>Vivian (A4)</t>
+  </si>
+  <si>
+    <t>Ralp (A5)</t>
+  </si>
+  <si>
+    <t>Jimy (A6)</t>
+  </si>
+  <si>
+    <t>Gavin (A7)</t>
+  </si>
+  <si>
+    <t>Maggie (A8)</t>
+  </si>
+  <si>
+    <t>JayZ (A9)</t>
+  </si>
+  <si>
+    <t>Parker (A10)</t>
+  </si>
+  <si>
+    <t>Singh (A11)</t>
+  </si>
+  <si>
+    <t>Jupiter (A12)</t>
+  </si>
+  <si>
+    <t>Kasi (A13)</t>
+  </si>
+  <si>
+    <t>Asah (A14)</t>
+  </si>
+  <si>
+    <t>Tyler (A15)</t>
+  </si>
+  <si>
+    <t>Mike (A16)</t>
   </si>
 </sst>
 </file>
@@ -369,8 +417,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G40" sqref="G40"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D49" sqref="D49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -606,10 +654,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B1"/>
+  <dimension ref="A1:B17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B31" sqref="A2:B31"/>
+    <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -624,6 +672,134 @@
       </c>
       <c r="B1" t="s">
         <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>12</v>
+      </c>
+      <c r="B8">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>13</v>
+      </c>
+      <c r="B9">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>14</v>
+      </c>
+      <c r="B10">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>15</v>
+      </c>
+      <c r="B11">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>16</v>
+      </c>
+      <c r="B12">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>17</v>
+      </c>
+      <c r="B13">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>18</v>
+      </c>
+      <c r="B14">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>19</v>
+      </c>
+      <c r="B15">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>20</v>
+      </c>
+      <c r="B16">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>21</v>
+      </c>
+      <c r="B17">
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>